<commit_message>
backup ngày 2025-09-23 (lần 3)
</commit_message>
<xml_diff>
--- a/backend/smoke_out/offers_export.xlsx
+++ b/backend/smoke_out/offers_export.xlsx
@@ -229,19 +229,19 @@
     <t>Ngày cập nhật</t>
   </si>
   <si>
-    <t>2025-09-22T12:52:20.273613</t>
-  </si>
-  <si>
-    <t>2025-09-22T12:52:20.276952</t>
-  </si>
-  <si>
-    <t>2025-09-22T12:52:20.278219</t>
-  </si>
-  <si>
-    <t>2025-09-22T12:52:20.279502</t>
-  </si>
-  <si>
-    <t>2025-09-22T12:52:20.280750</t>
+    <t>2025-09-23T13:37:31.130632</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:37:31.132284</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:37:31.133203</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:37:31.134036</t>
+  </si>
+  <si>
+    <t>2025-09-23T13:37:31.134926</t>
   </si>
   <si>
     <t>Mô tả chi tiết</t>

</xml_diff>